<commit_message>
fix: Update civilité options to include periods and adjust role determination logic in import functions
</commit_message>
<xml_diff>
--- a/public/models/commercial/commercial.xlsx
+++ b/public/models/commercial/commercial.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DEV-MBL\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DEV-MBL\Desktop\Projet\Wizi-learn-laravel\public\models\commercial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34F1CAED-22CC-4AF1-A24A-5ABD41376E39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC7589DA-3C9F-49E1-9508-BABEDD9EC71A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AD13FCCF-3CCE-4013-B31B-D6C2F6A2BB2A}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AD13FCCF-3CCE-4013-B31B-D6C2F6A2BB2A}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -29,14 +29,32 @@
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>Interlocuteur</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>nom</t>
+  </si>
+  <si>
+    <t>prénom</t>
+  </si>
+  <si>
+    <t>civilite</t>
+  </si>
+  <si>
+    <t>tel</t>
+  </si>
+  <si>
+    <t>adresse</t>
   </si>
 </sst>
 </file>
@@ -396,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DCFD262-1E37-4925-879A-06DE2C408225}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -407,9 +425,24 @@
     <col min="1" max="1" width="21.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>